<commit_message>
[16857]-[17081]: chỉ chuyến đã được lái xe nhận
</commit_message>
<xml_diff>
--- a/bangluudulieu_tamthoi.xlsx
+++ b/bangluudulieu_tamthoi.xlsx
@@ -507,8 +507,8 @@
   </sheetPr>
   <dimension ref="A1:O337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="L137" sqref="L137"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -556,7 +556,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>auto1446</t>
+          <t>2024AUTO1480</t>
         </is>
       </c>
     </row>
@@ -580,7 +580,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -592,7 +592,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>/Content/themes/img/BlueCar.png</t>
+          <t>/Content/themes/img/RedCar.png</t>
         </is>
       </c>
     </row>
@@ -604,27 +604,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>//*[@class='table table-hover table-bordered']/tbody/tr[27]/td[1]/img</t>
+          <t>//*[@class='table table-hover table-bordered']/tbody/tr[9]/td[1]/img</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>//*[@class='table table-hover table-bordered']/tbody/tr[27]/td[2]</t>
+          <t>//*[@class='table table-hover table-bordered']/tbody/tr[9]/td[2]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>//*[@class='table table-hover table-bordered']/tbody/tr[27]/td[3]</t>
+          <t>//*[@class='table table-hover table-bordered']/tbody/tr[9]/td[3]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>//*[@class='table table-hover table-bordered']/tbody/tr[27]/td[4]</t>
+          <t>//*[@class='table table-hover table-bordered']/tbody/tr[9]/td[4]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>//*[@class='table table-hover table-bordered']/tbody/tr[27]/td[5]</t>
+          <t>//*[@class='table table-hover table-bordered']/tbody/tr[9]/td[5]</t>
         </is>
       </c>
     </row>
@@ -635,11 +635,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1455</v>
+        <v>1480</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_04072025_1455</t>
+          <t>_09072025_1480</t>
         </is>
       </c>
     </row>
@@ -652,7 +652,7 @@
       <c r="B8" s="2" t="n"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>15A26900</t>
+          <t>15A32281</t>
         </is>
       </c>
     </row>
@@ -664,12 +664,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>219</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>219</t>
         </is>
       </c>
     </row>
@@ -681,12 +681,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>P. Hưng Đạo, Q. Dương Kinh, TP. Hải Phòng</t>
+          <t>173, Văn Cao, P. Đằng Giang, Q. Ngô Quyền, TP. Hải Phòng</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>P. Hưng Đạo, Q. Dương Kinh, TP. Hải Phòng</t>
+          <t>171, Văn Cao, P. Đằng Giang, Q. Ngô Quyền, TP. Hải Phòng</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>20.79632</t>
+          <t>20.83662</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>106.6786</t>
+          <t>106.7012</t>
         </is>
       </c>
     </row>
@@ -722,12 +722,12 @@
       </c>
       <c r="B13" s="7" t="inlineStr">
         <is>
-          <t>01:06:17</t>
+          <t>01:05:47</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>01:06:17</t>
+          <t>01:05:47</t>
         </is>
       </c>
     </row>
@@ -756,12 +756,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>5 chỗ Nguyễn Gia - Zinger</t>
+          <t>5 chỗ Nguyễn Gia - VIOS</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5 chỗ Nguyễn Gia - Zinger</t>
+          <t>5 chỗ Nguyễn Gia - VIOS</t>
         </is>
       </c>
     </row>
@@ -829,12 +829,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Phạm Thanh Tuấn</t>
+          <t>TRẦN ĐỨC TIẾN</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Phạm Thanh Tuấn</t>
+          <t>TRẦN ĐỨC TIẾN</t>
         </is>
       </c>
     </row>
@@ -846,12 +846,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0981828568</t>
+          <t>0904074490</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0981828568</t>
+          <t>0904074490</t>
         </is>
       </c>
     </row>
@@ -863,7 +863,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Không kết nối</t>
+          <t>Kết nối</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2100001448</t>
+          <t>2100001478</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -986,7 +986,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Auto1450</t>
+          <t>Auto1469</t>
         </is>
       </c>
     </row>
@@ -998,7 +998,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Auto_1451</t>
+          <t>Auto_1470</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>auto1454</t>
+          <t>auto1473</t>
         </is>
       </c>
     </row>
@@ -1022,7 +1022,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Auto_ThongBao_1455</t>
+          <t>Auto_ThongBao_1474</t>
         </is>
       </c>
     </row>
@@ -1063,15 +1063,15 @@
     <row r="42">
       <c r="B42" t="inlineStr">
         <is>
-          <t>Tìm kiếm</t>
+          <t>Thêm mới</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>Có dữ liệu tìm kiếm hàng đầu tiên
-(Hiển thị Tên lái xe)</t>
+          <t>Hiển thị message: "Thêm mới xe thành công."
+(biển số tạo ở ô ghi chú)</t>
         </is>
       </c>
     </row>
@@ -1134,7 +1134,7 @@
     <row r="47" ht="15.75" customHeight="1" s="19">
       <c r="B47" t="inlineStr">
         <is>
-          <t>01:00</t>
+          <t>09:34:32</t>
         </is>
       </c>
       <c r="F47" s="11" t="n">
@@ -1511,7 +1511,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77">
@@ -1522,7 +1522,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="81">
       <c r="B81" t="n">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="82">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>238</t>
+          <t>237</t>
         </is>
       </c>
     </row>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="B133" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0 ₫</t>
         </is>
       </c>
       <c r="C133" s="8" t="inlineStr">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Test tự động đặt cuốc</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">

</xml_diff>

<commit_message>
[BAEX-17199]: style css 11
</commit_message>
<xml_diff>
--- a/bangluudulieu_tamthoi.xlsx
+++ b/bangluudulieu_tamthoi.xlsx
@@ -507,8 +507,8 @@
   </sheetPr>
   <dimension ref="A1:O337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="H126" sqref="H126"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -556,7 +556,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>auto1795</t>
+          <t>18H03460</t>
         </is>
       </c>
     </row>
@@ -604,27 +604,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>//*[@class='table table-hover table-bordered']/tbody/tr[3]/td[1]/img</t>
+          <t>//*[@class='table table-hover table-bordered']/tbody/tr[2]/td[1]/img</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>//*[@class='table table-hover table-bordered']/tbody/tr[3]/td[2]</t>
+          <t>//*[@class='table table-hover table-bordered']/tbody/tr[2]/td[2]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>//*[@class='table table-hover table-bordered']/tbody/tr[3]/td[3]</t>
+          <t>//*[@class='table table-hover table-bordered']/tbody/tr[2]/td[3]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>//*[@class='table table-hover table-bordered']/tbody/tr[3]/td[4]</t>
+          <t>//*[@class='table table-hover table-bordered']/tbody/tr[2]/td[4]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>//*[@class='table table-hover table-bordered']/tbody/tr[3]/td[5]</t>
+          <t>//*[@class='table table-hover table-bordered']/tbody/tr[2]/td[5]</t>
         </is>
       </c>
     </row>
@@ -635,11 +635,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1796</v>
+        <v>2177</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_11082025_1796</t>
+          <t>_10102025_2177</t>
         </is>
       </c>
     </row>
@@ -652,7 +652,7 @@
       <c r="B8" s="2" t="n"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>15A34431</t>
+          <t>15A26857</t>
         </is>
       </c>
     </row>
@@ -664,12 +664,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>164</t>
+          <t>205</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>164</t>
+          <t>205</t>
         </is>
       </c>
     </row>
@@ -681,12 +681,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bùi Hướng Thành, X. Minh Tân, H. Kiến Thụy, TP. Hải Phòng</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Bùi Hướng Thành, X. Minh Tân, H. Kiến Thụy, TP. Hải Phòng</t>
+          <t>11, Bạch Đằng, P. Thủy Nguyên, , TP. Hải Phòng</t>
         </is>
       </c>
     </row>
@@ -698,7 +693,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>20.75425</t>
+          <t>20.91827</t>
         </is>
       </c>
     </row>
@@ -710,7 +705,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>106.6782</t>
+          <t>106.6759</t>
         </is>
       </c>
     </row>
@@ -722,12 +717,12 @@
       </c>
       <c r="B13" s="7" t="inlineStr">
         <is>
-          <t>01:35:57</t>
+          <t>08:41:38</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>01:35:57</t>
+          <t>08:41:38</t>
         </is>
       </c>
     </row>
@@ -739,12 +734,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -756,12 +751,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>4 chỗ Nguyễn Gia - KIA</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>4 chỗ Nguyễn Gia - KIA</t>
+          <t>5 chỗ Nguyễn Gia - VIOS</t>
         </is>
       </c>
     </row>
@@ -781,11 +771,6 @@
           <t>Sẵn sàng</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Sẵn sàng</t>
-        </is>
-      </c>
     </row>
     <row r="17" ht="18.75" customHeight="1" s="19">
       <c r="A17" s="5" t="inlineStr">
@@ -795,7 +780,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0 (TTĐH:0;App:0;Vẫy:0)</t>
+          <t>1 (TTĐH:1;App:0;Vẫy:0)</t>
         </is>
       </c>
     </row>
@@ -810,11 +795,6 @@
           <t>0</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
     </row>
     <row r="19" ht="18.75" customHeight="1" s="19">
       <c r="A19" s="4" t="inlineStr">
@@ -829,12 +809,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Lê Văn hai</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Lê Văn hai</t>
+          <t>HOÀNG VĂN NHÂN</t>
         </is>
       </c>
     </row>
@@ -846,12 +821,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0932781986</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>0932781986</t>
+          <t>0906041039</t>
         </is>
       </c>
     </row>
@@ -863,7 +833,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Kết nối</t>
+          <t>Không kết nối</t>
         </is>
       </c>
     </row>
@@ -875,12 +845,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>607030</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>607030</t>
+          <t>507121</t>
         </is>
       </c>
     </row>
@@ -892,12 +857,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Auto_KM_Chung1768</t>
+          <t>Auto_KM_Chung2163</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Auto_KM_Rieng1770</t>
+          <t>Auto_KM_Rieng2164</t>
         </is>
       </c>
     </row>
@@ -909,7 +874,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2100001785</t>
+          <t>2100002074</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -926,7 +891,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Auto_CaiAppMoi1771</t>
+          <t>Auto_CaiAppMoi2141</t>
         </is>
       </c>
     </row>
@@ -938,7 +903,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Auto_account_292</t>
+          <t>Auto_account_2051</t>
         </is>
       </c>
     </row>
@@ -950,7 +915,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Auto_group_293</t>
+          <t>Auto_group_2052</t>
         </is>
       </c>
     </row>
@@ -962,7 +927,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Auto_customer_1288</t>
+          <t>Auto_customer_2143</t>
         </is>
       </c>
     </row>
@@ -974,7 +939,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Auto_name_partner_1178</t>
+          <t>Auto_name_partner_2165</t>
         </is>
       </c>
     </row>
@@ -986,7 +951,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Auto1787</t>
+          <t>Auto2167</t>
         </is>
       </c>
     </row>
@@ -998,7 +963,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Auto_1788</t>
+          <t>Auto_2177</t>
         </is>
       </c>
     </row>
@@ -1010,7 +975,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>auto1791</t>
+          <t>auto2150</t>
         </is>
       </c>
     </row>
@@ -1022,7 +987,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Auto_ThongBao_1796</t>
+          <t>Auto_ThongBao_2152</t>
         </is>
       </c>
     </row>
@@ -1034,7 +999,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Auto_ThongBaoV2_1193</t>
+          <t>Auto_ThongBaoV2_2153</t>
         </is>
       </c>
     </row>
@@ -1060,17 +1025,25 @@
         <v>0</v>
       </c>
     </row>
+    <row r="37">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Auto_2128</t>
+        </is>
+      </c>
+    </row>
     <row r="42">
       <c r="B42" t="inlineStr">
         <is>
-          <t>Xuất hóa đơn - Lưu</t>
+          <t>Xuất excel</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>Hiển thị message: "Lưu thông tin thành công!"</t>
+          <t>1. Tải file Excel về máy
+(Chỉ check tải, không check dữ liệu)</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1106,7 @@
     <row r="47" ht="15.75" customHeight="1" s="19">
       <c r="B47" t="inlineStr">
         <is>
-          <t>08:35:54</t>
+          <t>16:31:26</t>
         </is>
       </c>
       <c r="F47" s="11" t="n">
@@ -1283,7 +1256,7 @@
     </row>
     <row r="60">
       <c r="B60" t="n">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="F60" t="n">
         <v>100000</v>
@@ -1293,8 +1266,10 @@
       </c>
     </row>
     <row r="61">
-      <c r="B61" t="n">
-        <v>2</v>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="F61" t="n">
         <v>18</v>
@@ -1380,7 +1355,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="F66" t="n">
         <v>120000</v>
@@ -1510,7 +1485,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77">
@@ -1521,7 +1496,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>10</t>
         </is>
       </c>
     </row>
@@ -1549,12 +1524,12 @@
     </row>
     <row r="80">
       <c r="B80" t="n">
-        <v>0</v>
+        <v>528</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="n">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="82">
@@ -1601,7 +1576,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0</v>
+        <v>528</v>
       </c>
     </row>
     <row r="87">
@@ -1612,7 +1587,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>235</t>
+          <t>528</t>
         </is>
       </c>
     </row>
@@ -1800,6 +1775,13 @@
         <v>4348000</v>
       </c>
     </row>
+    <row r="110">
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>C:/Users/truongtq.BA/PycharmProjects/pythonProject/s_taxi/file/</t>
+        </is>
+      </c>
+    </row>
     <row r="120">
       <c r="A120" s="8" t="inlineStr">
         <is>
@@ -1835,22 +1817,22 @@
     <row r="121">
       <c r="A121" s="8" t="inlineStr">
         <is>
-          <t>Tên khuyến mại</t>
+          <t>Công ty</t>
         </is>
       </c>
       <c r="B121" s="8" t="inlineStr">
         <is>
-          <t>Km 30%</t>
+          <t>G7 Taxi Hà Nội</t>
         </is>
       </c>
       <c r="C121" s="8" t="inlineStr">
         <is>
-          <t>Tên khuyến mại</t>
+          <t>Công ty</t>
         </is>
       </c>
       <c r="D121" s="8" t="inlineStr">
         <is>
-          <t>KM tháng 6 theo %</t>
+          <t>G7 Taxi Hà Nội</t>
         </is>
       </c>
       <c r="E121" s="8" t="inlineStr">
@@ -1867,22 +1849,22 @@
     <row r="122">
       <c r="A122" s="8" t="inlineStr">
         <is>
-          <t>Tổng tiền đã khuyến mại</t>
+          <t>Tổng số tin nhắn</t>
         </is>
       </c>
       <c r="B122" s="8" t="inlineStr">
         <is>
-          <t>465.000 ₫</t>
+          <t>21</t>
         </is>
       </c>
       <c r="C122" s="8" t="inlineStr">
         <is>
-          <t>Tổng tiền đã khuyến mại</t>
+          <t>Tổng số tin nhắn</t>
         </is>
       </c>
       <c r="D122" s="8" t="inlineStr">
         <is>
-          <t>701.000 ₫</t>
+          <t>21</t>
         </is>
       </c>
       <c r="E122" s="8" t="inlineStr">
@@ -1899,22 +1881,22 @@
     <row r="123">
       <c r="A123" s="8" t="inlineStr">
         <is>
-          <t>Tổng số khuyến mại đã sử dụng</t>
+          <t>Tin đăng ký</t>
         </is>
       </c>
       <c r="B123" s="8" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C123" s="8" t="inlineStr">
         <is>
-          <t>Tổng số khuyến mại đã sử dụng</t>
+          <t>Tin đăng ký</t>
         </is>
       </c>
       <c r="D123" s="8" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>16</t>
         </is>
       </c>
       <c r="E123" s="8" t="inlineStr">
@@ -1931,18 +1913,22 @@
     <row r="124">
       <c r="A124" s="8" t="inlineStr">
         <is>
-          <t>12/2024</t>
-        </is>
-      </c>
-      <c r="B124" s="8" t="inlineStr"/>
+          <t>Tin giới thiệu</t>
+        </is>
+      </c>
+      <c r="B124" s="8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="C124" s="8" t="inlineStr">
         <is>
-          <t>12/2024</t>
+          <t>Tin đi ngay</t>
         </is>
       </c>
       <c r="D124" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E124" s="8" t="inlineStr">
@@ -1959,18 +1945,22 @@
     <row r="125">
       <c r="A125" s="8" t="inlineStr">
         <is>
-          <t>01/2025</t>
-        </is>
-      </c>
-      <c r="B125" s="8" t="inlineStr"/>
+          <t>Tin đường dài</t>
+        </is>
+      </c>
+      <c r="B125" s="8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="C125" s="8" t="inlineStr">
         <is>
-          <t>01/2025</t>
+          <t>Tin đường dài</t>
         </is>
       </c>
       <c r="D125" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E125" s="8" t="inlineStr">
@@ -1987,18 +1977,22 @@
     <row r="126">
       <c r="A126" s="8" t="inlineStr">
         <is>
-          <t>02/2025</t>
-        </is>
-      </c>
-      <c r="B126" s="8" t="inlineStr"/>
+          <t>Tin sân bay</t>
+        </is>
+      </c>
+      <c r="B126" s="8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="C126" s="8" t="inlineStr">
         <is>
-          <t>02/2025</t>
+          <t>Tin sân bay</t>
         </is>
       </c>
       <c r="D126" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E126" s="8" t="inlineStr">
@@ -2015,18 +2009,22 @@
     <row r="127">
       <c r="A127" s="8" t="inlineStr">
         <is>
-          <t>03/2025</t>
-        </is>
-      </c>
-      <c r="B127" s="8" t="inlineStr"/>
+          <t>Tin khác</t>
+        </is>
+      </c>
+      <c r="B127" s="8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="C127" s="8" t="inlineStr">
         <is>
-          <t>03/2025</t>
+          <t>Tin khác</t>
         </is>
       </c>
       <c r="D127" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E127" s="8" t="inlineStr">
@@ -2043,18 +2041,22 @@
     <row r="128">
       <c r="A128" s="8" t="inlineStr">
         <is>
-          <t>04/2025</t>
-        </is>
-      </c>
-      <c r="B128" s="8" t="inlineStr"/>
+          <t>Tin OTP mã pin</t>
+        </is>
+      </c>
+      <c r="B128" s="8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="C128" s="8" t="inlineStr">
         <is>
-          <t>04/2025</t>
+          <t>Tin OTP mã pin</t>
         </is>
       </c>
       <c r="D128" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E128" s="8" t="inlineStr">
@@ -2069,127 +2071,39 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="8" t="inlineStr">
-        <is>
-          <t>05/2025</t>
-        </is>
-      </c>
+      <c r="A129" s="8" t="inlineStr"/>
       <c r="B129" s="8" t="inlineStr"/>
-      <c r="C129" s="8" t="inlineStr">
-        <is>
-          <t>05/2025</t>
-        </is>
-      </c>
-      <c r="D129" s="8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E129" s="8" t="inlineStr">
-        <is>
-          <t>J5</t>
-        </is>
-      </c>
-      <c r="F129" s="8" t="inlineStr">
-        <is>
-          <t>J6</t>
-        </is>
-      </c>
+      <c r="C129" s="8" t="inlineStr"/>
+      <c r="D129" s="8" t="inlineStr"/>
+      <c r="E129" s="8" t="inlineStr"/>
+      <c r="F129" s="8" t="inlineStr"/>
     </row>
     <row r="130">
-      <c r="A130" s="8" t="inlineStr">
-        <is>
-          <t>06/2025</t>
-        </is>
-      </c>
+      <c r="A130" s="8" t="inlineStr"/>
       <c r="B130" s="8" t="inlineStr"/>
-      <c r="C130" s="8" t="inlineStr">
-        <is>
-          <t>06/2025</t>
-        </is>
-      </c>
-      <c r="D130" s="8" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="E130" s="8" t="inlineStr">
-        <is>
-          <t>K5</t>
-        </is>
-      </c>
-      <c r="F130" s="8" t="inlineStr">
-        <is>
-          <t>K6</t>
-        </is>
-      </c>
+      <c r="C130" s="8" t="inlineStr"/>
+      <c r="D130" s="8" t="inlineStr"/>
+      <c r="E130" s="8" t="inlineStr"/>
+      <c r="F130" s="8" t="inlineStr"/>
     </row>
     <row r="131">
-      <c r="A131" s="8" t="inlineStr">
-        <is>
-          <t>07/2025</t>
-        </is>
-      </c>
-      <c r="B131" s="8" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="C131" s="8" t="inlineStr">
-        <is>
-          <t>07/2025</t>
-        </is>
-      </c>
-      <c r="D131" s="8" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E131" s="8" t="inlineStr">
-        <is>
-          <t>L5</t>
-        </is>
-      </c>
-      <c r="F131" s="8" t="inlineStr">
-        <is>
-          <t>L6</t>
-        </is>
-      </c>
+      <c r="A131" s="8" t="inlineStr"/>
+      <c r="B131" s="8" t="inlineStr"/>
+      <c r="C131" s="8" t="inlineStr"/>
+      <c r="D131" s="8" t="inlineStr"/>
+      <c r="E131" s="8" t="inlineStr"/>
+      <c r="F131" s="8" t="inlineStr"/>
     </row>
     <row r="132">
-      <c r="A132" s="8" t="inlineStr">
-        <is>
-          <t>08/2025</t>
-        </is>
-      </c>
+      <c r="A132" s="8" t="inlineStr"/>
       <c r="B132" s="8" t="inlineStr"/>
-      <c r="C132" s="8" t="inlineStr">
-        <is>
-          <t>08/2025</t>
-        </is>
-      </c>
-      <c r="D132" s="8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E132" s="8" t="inlineStr">
-        <is>
-          <t>M5</t>
-        </is>
-      </c>
-      <c r="F132" s="8" t="inlineStr">
-        <is>
-          <t>M6</t>
-        </is>
-      </c>
+      <c r="C132" s="8" t="inlineStr"/>
+      <c r="D132" s="8" t="inlineStr"/>
+      <c r="E132" s="8" t="inlineStr"/>
+      <c r="F132" s="8" t="inlineStr"/>
     </row>
     <row r="133">
-      <c r="A133" s="8" t="inlineStr">
-        <is>
-          <t>09/2025</t>
-        </is>
-      </c>
+      <c r="A133" s="8" t="inlineStr"/>
       <c r="B133" s="8" t="inlineStr"/>
       <c r="C133" s="8" t="inlineStr"/>
       <c r="D133" s="8" t="inlineStr"/>
@@ -2197,11 +2111,7 @@
       <c r="F133" s="8" t="inlineStr"/>
     </row>
     <row r="134">
-      <c r="A134" s="8" t="inlineStr">
-        <is>
-          <t>10/2025</t>
-        </is>
-      </c>
+      <c r="A134" s="8" t="inlineStr"/>
       <c r="B134" s="8" t="inlineStr"/>
       <c r="C134" s="8" t="inlineStr"/>
       <c r="D134" s="8" t="inlineStr"/>
@@ -2209,11 +2119,7 @@
       <c r="F134" s="8" t="inlineStr"/>
     </row>
     <row r="135">
-      <c r="A135" s="8" t="inlineStr">
-        <is>
-          <t>11/2025</t>
-        </is>
-      </c>
+      <c r="A135" s="8" t="inlineStr"/>
       <c r="B135" s="8" t="inlineStr"/>
       <c r="C135" s="8" t="inlineStr"/>
       <c r="D135" s="8" t="inlineStr"/>
@@ -2221,11 +2127,7 @@
       <c r="F135" s="8" t="inlineStr"/>
     </row>
     <row r="136">
-      <c r="A136" s="8" t="inlineStr">
-        <is>
-          <t>12/2025</t>
-        </is>
-      </c>
+      <c r="A136" s="8" t="inlineStr"/>
       <c r="B136" s="8" t="inlineStr"/>
       <c r="C136" s="8" t="inlineStr"/>
       <c r="D136" s="8" t="inlineStr"/>
@@ -2233,11 +2135,7 @@
       <c r="F136" s="8" t="inlineStr"/>
     </row>
     <row r="137">
-      <c r="A137" s="8" t="inlineStr">
-        <is>
-          <t>01/2026</t>
-        </is>
-      </c>
+      <c r="A137" s="8" t="inlineStr"/>
       <c r="B137" s="8" t="inlineStr"/>
       <c r="C137" s="8" t="inlineStr"/>
       <c r="D137" s="8" t="inlineStr"/>
@@ -2245,11 +2143,7 @@
       <c r="F137" s="8" t="inlineStr"/>
     </row>
     <row r="138">
-      <c r="A138" s="8" t="inlineStr">
-        <is>
-          <t>02/2026</t>
-        </is>
-      </c>
+      <c r="A138" s="8" t="inlineStr"/>
       <c r="B138" s="8" t="inlineStr"/>
       <c r="C138" s="8" t="inlineStr"/>
       <c r="D138" s="8" t="inlineStr"/>
@@ -2257,11 +2151,7 @@
       <c r="F138" s="8" t="inlineStr"/>
     </row>
     <row r="139">
-      <c r="A139" s="8" t="inlineStr">
-        <is>
-          <t>03/2026</t>
-        </is>
-      </c>
+      <c r="A139" s="8" t="inlineStr"/>
       <c r="B139" s="8" t="inlineStr"/>
       <c r="C139" s="8" t="inlineStr"/>
       <c r="D139" s="8" t="inlineStr"/>
@@ -2269,11 +2159,7 @@
       <c r="F139" s="8" t="inlineStr"/>
     </row>
     <row r="140">
-      <c r="A140" s="8" t="inlineStr">
-        <is>
-          <t>04/2026</t>
-        </is>
-      </c>
+      <c r="A140" s="8" t="inlineStr"/>
       <c r="B140" s="8" t="inlineStr"/>
       <c r="C140" s="8" t="inlineStr"/>
       <c r="D140" s="8" t="inlineStr"/>
@@ -2281,11 +2167,7 @@
       <c r="F140" s="8" t="inlineStr"/>
     </row>
     <row r="141">
-      <c r="A141" s="8" t="inlineStr">
-        <is>
-          <t>05/2026</t>
-        </is>
-      </c>
+      <c r="A141" s="8" t="inlineStr"/>
       <c r="B141" s="8" t="inlineStr"/>
       <c r="C141" s="8" t="inlineStr"/>
       <c r="D141" s="8" t="inlineStr"/>
@@ -2367,17 +2249,22 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>07/08</t>
+          <t>04/09</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>HTTT cuốc</t>
+          <t>04/09</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Tiền mặt</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -2394,12 +2281,17 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>08/08</t>
+          <t>05/09</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Ghi chú</t>
+          <t>05/09</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -2416,17 +2308,17 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>09/08</t>
+          <t>06/09</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Km có khách (GPS)</t>
+          <t>06/09</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -2443,12 +2335,12 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10/08</t>
+          <t>07/09</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Biển số xe (GPS)</t>
+          <t>07/09</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -2470,12 +2362,12 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>11/08</t>
+          <t>08/09</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Số hiệu (GPS)</t>
+          <t>08/09</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -2497,12 +2389,12 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>12/08</t>
+          <t>09/09</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Loại xe (GPS)</t>
+          <t>09/09</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -2522,9 +2414,9 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>13/08</t>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -2549,9 +2441,9 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>14/08</t>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -2576,11 +2468,6 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>15/08</t>
-        </is>
-      </c>
       <c r="C159" t="inlineStr">
         <is>
           <t>Thời gian đón khách (Đồng hồ - GPS)</t>
@@ -2603,11 +2490,6 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>16/08</t>
-        </is>
-      </c>
       <c r="C160" t="inlineStr">
         <is>
           <t>Thời gian trả khách (Đồng hồ - GPS)</t>
@@ -2629,66 +2511,62 @@
         </is>
       </c>
     </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>17/08</t>
-        </is>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>18/08</t>
-        </is>
-      </c>
-    </row>
     <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>19/08</t>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Xem</t>
         </is>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>20/08</t>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Xem</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>21/08</t>
+          <t>Cuốc khách GPS</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Xem</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>22/08</t>
+          <t>Lộ trình GPS</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Xem </t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>23/08</t>
+          <t>22/01</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>24/08</t>
+          <t>23/01</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>25/08</t>
+          <t>24/01</t>
         </is>
       </c>
     </row>
@@ -2699,9 +2577,13 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>400000</v>
-      </c>
-      <c r="D170" s="16" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="D170" s="16" t="inlineStr">
+        <is>
+          <t>Không tìm thấy thẻ</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -2710,7 +2592,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>400000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172">
@@ -2720,12 +2602,16 @@
         </is>
       </c>
       <c r="B172" s="17" t="n">
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="C172" t="n">
         <v>2</v>
       </c>
-      <c r="D172" s="16" t="n"/>
+      <c r="D172" s="16" t="inlineStr">
+        <is>
+          <t>Không tìm thấy thẻ</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="17" t="inlineStr">
@@ -2760,7 +2646,7 @@
         </is>
       </c>
       <c r="B175" s="17" t="n">
-        <v>-400000</v>
+        <v>0</v>
       </c>
       <c r="C175" t="n">
         <v>1</v>
@@ -2773,7 +2659,7 @@
         </is>
       </c>
       <c r="B176" s="17" t="n">
-        <v>10000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177">
@@ -2783,12 +2669,16 @@
         </is>
       </c>
       <c r="B177" s="17" t="n">
-        <v>-400000</v>
+        <v>0</v>
       </c>
       <c r="C177" t="n">
         <v>1</v>
       </c>
-      <c r="D177" s="16" t="n"/>
+      <c r="D177" s="16" t="inlineStr">
+        <is>
+          <t>Không tìm thấy thẻ</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="17" t="inlineStr">
@@ -2797,7 +2687,7 @@
         </is>
       </c>
       <c r="B178" s="17" t="n">
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="C178" t="n">
         <v>2</v>
@@ -2822,8 +2712,10 @@
           <t>thẻ sau4: 7.7.5 Số tiền 1 serial</t>
         </is>
       </c>
-      <c r="B180" s="17" t="n">
-        <v>0</v>
+      <c r="B180" s="17" t="inlineStr">
+        <is>
+          <t>151000</t>
+        </is>
       </c>
       <c r="C180" t="n">
         <v>1</v>
@@ -2849,7 +2741,7 @@
         </is>
       </c>
       <c r="B182" s="17" t="n">
-        <v>0</v>
+        <v>151000</v>
       </c>
       <c r="C182" t="n">
         <v>3</v>
@@ -2861,17 +2753,15 @@
           <t>thẻ sau4: 7.7.5 Số tiền hợp đồng</t>
         </is>
       </c>
-      <c r="B183" s="17" t="n">
-        <v>0</v>
+      <c r="B183" s="17" t="inlineStr">
+        <is>
+          <t>151000</t>
+        </is>
       </c>
       <c r="C183" t="n">
         <v>4</v>
       </c>
-      <c r="D183" s="16" t="inlineStr">
-        <is>
-          <t>Không tìm thấy thẻ</t>
-        </is>
-      </c>
+      <c r="D183" s="16" t="n"/>
     </row>
     <row r="184">
       <c r="B184" t="n">
@@ -2896,11 +2786,6 @@
           <t>Tên cấu hình(10.6.3)</t>
         </is>
       </c>
-      <c r="B190" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -2908,11 +2793,7 @@
           <t>Mã serial(7.7.4)</t>
         </is>
       </c>
-      <c r="B191" s="18" t="inlineStr">
-        <is>
-          <t>8888999966949781</t>
-        </is>
-      </c>
+      <c r="B191" s="18" t="n"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -2920,11 +2801,6 @@
           <t>Mất bản ghi (7.7.4)</t>
         </is>
       </c>
-      <c r="B192" t="inlineStr">
-        <is>
-          <t>Đã mất bản ghi</t>
-        </is>
-      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -2932,11 +2808,6 @@
           <t>Mã phiếu chôt(7.7.4)</t>
         </is>
       </c>
-      <c r="B193" t="inlineStr">
-        <is>
-          <t>G7_0009163</t>
-        </is>
-      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -2944,10 +2815,8 @@
           <t>Tổng tiền chốt(7.7.4)</t>
         </is>
       </c>
-      <c r="B194" t="inlineStr">
-        <is>
-          <t>214.000</t>
-        </is>
+      <c r="B194" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -2956,11 +2825,6 @@
           <t>Mã công nợ(7.7.5)</t>
         </is>
       </c>
-      <c r="B196" t="inlineStr">
-        <is>
-          <t>G7_0009163</t>
-        </is>
-      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -2968,11 +2832,6 @@
           <t>Mã hợp đồng(7.7.5)</t>
         </is>
       </c>
-      <c r="B197" t="inlineStr">
-        <is>
-          <t>G7_0009</t>
-        </is>
-      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -2980,11 +2839,7 @@
           <t>T.gian chốt(7.7.5)</t>
         </is>
       </c>
-      <c r="B198" s="2" t="inlineStr">
-        <is>
-          <t>16:01:26 - 12/05/2025</t>
-        </is>
-      </c>
+      <c r="B198" s="2" t="n"/>
       <c r="C198" s="2" t="n"/>
     </row>
     <row r="199">
@@ -2993,10 +2848,8 @@
           <t>S.tiền nợ chốt(7.7.5)</t>
         </is>
       </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>214.000 ₫</t>
-        </is>
+      <c r="B199" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="200">
@@ -3005,11 +2858,6 @@
           <t>T.thái phiếu(7.7.5)</t>
         </is>
       </c>
-      <c r="B200" t="inlineStr">
-        <is>
-          <t>Đã chốt</t>
-        </is>
-      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -3017,11 +2865,6 @@
           <t>T.thái t.toán(7.7.5)</t>
         </is>
       </c>
-      <c r="B201" t="inlineStr">
-        <is>
-          <t>Chưa thanh toán</t>
-        </is>
-      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -3029,11 +2872,6 @@
           <t>Người chốt(7.7.5)</t>
         </is>
       </c>
-      <c r="B202" t="inlineStr">
-        <is>
-          <t>autoba</t>
-        </is>
-      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -3048,11 +2886,6 @@
           <t>Mã công nợ(7.7.6)</t>
         </is>
       </c>
-      <c r="B205" t="inlineStr">
-        <is>
-          <t>G7_0009163</t>
-        </is>
-      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -3060,11 +2893,6 @@
           <t>Mã hợp đồng(7.7.6)</t>
         </is>
       </c>
-      <c r="B206" t="inlineStr">
-        <is>
-          <t>G7_0009</t>
-        </is>
-      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -3072,11 +2900,7 @@
           <t>Thời gian thao tác(7.7.6)</t>
         </is>
       </c>
-      <c r="B207" s="2" t="inlineStr">
-        <is>
-          <t>16:1:26 12/5/2025</t>
-        </is>
-      </c>
+      <c r="B207" s="2" t="n"/>
       <c r="C207" s="2" t="n"/>
     </row>
     <row r="208">
@@ -3085,11 +2909,6 @@
           <t>Người thao tác(7.7.6)</t>
         </is>
       </c>
-      <c r="B208" t="inlineStr">
-        <is>
-          <t>autoba</t>
-        </is>
-      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -3097,10 +2916,8 @@
           <t>Tổng nợ(7.7.6)</t>
         </is>
       </c>
-      <c r="B209" t="inlineStr">
-        <is>
-          <t>214.000 ₫</t>
-        </is>
+      <c r="B209" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="210">
@@ -3109,11 +2926,6 @@
           <t>Loại thao tác(7.7.6)</t>
         </is>
       </c>
-      <c r="B210" t="inlineStr">
-        <is>
-          <t>Chốt</t>
-        </is>
-      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -3415,6 +3227,47 @@
       <c r="A238" t="inlineStr">
         <is>
           <t>Mất thẻ(7.7.3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Cho phép tạo</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="B251" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Không dữ liệu</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="B253" t="n">
+        <v>142000</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="B254" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="B255" t="n">
+        <v>2964</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="B256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chờ xác nhận, </t>
         </is>
       </c>
     </row>

</xml_diff>